<commit_message>
Add: screenshots of project and updated rubric
</commit_message>
<xml_diff>
--- a/DGL123-CodingRubric-finalproject-redjinator.xlsx
+++ b/DGL123-CodingRubric-finalproject-redjinator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\XAMPP\htdocs\Git\finalproject-php-Redjinator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A70072E4-2A9B-43B8-80EF-B4CB067A4364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68331F45-EAEE-4EB1-9B3A-438BCFCD0423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45" yWindow="45" windowWidth="17115" windowHeight="20910" xr2:uid="{CBF547A3-9D43-4F4A-A93D-3939F8DAC589}"/>
+    <workbookView xWindow="45" yWindow="45" windowWidth="22665" windowHeight="20910" xr2:uid="{CBF547A3-9D43-4F4A-A93D-3939F8DAC589}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -706,8 +706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFE407B3-376B-134C-820F-A035EA155628}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -774,7 +774,7 @@
         <v>21</v>
       </c>
       <c r="F4" s="16">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="1" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.25">
@@ -911,7 +911,7 @@
       <c r="E12" s="27"/>
       <c r="F12" s="12">
         <f>SUM(F4:F8)</f>
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>